<commit_message>
harmonizing code for all surveys but nfhs5
</commit_message>
<xml_diff>
--- a/District_Changes.xlsx
+++ b/District_Changes.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill.sharepoint.com/sites/PROSPERED_Group/Shared Documents/General/CIHR RSBY India/data/Linking code and CSVs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="511" documentId="8_{B95B0D2E-E9D4-8740-A922-149F5228A517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E63F870-C737-3A44-8AB9-F472E2179F25}"/>
+  <xr:revisionPtr revIDLastSave="658" documentId="8_{B95B0D2E-E9D4-8740-A922-149F5228A517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C4F2AE9-04FA-E840-9224-79CFA44E1815}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="500" windowWidth="33620" windowHeight="19380" xr2:uid="{D1D00CCF-82AB-6D4D-9728-F84D718C5775}"/>
+    <workbookView xWindow="2400" yWindow="1620" windowWidth="33620" windowHeight="19380" xr2:uid="{D1D00CCF-82AB-6D4D-9728-F84D718C5775}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="322">
   <si>
     <t>State</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Dima Hasao</t>
   </si>
   <si>
-    <t>North Cacha Hills</t>
-  </si>
-  <si>
     <t>Biswanath</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>Sukma</t>
   </si>
   <si>
-    <t>Dantewanda</t>
-  </si>
-  <si>
     <t>Surajpur</t>
   </si>
   <si>
@@ -402,9 +396,6 @@
     <t>Pratapgarh</t>
   </si>
   <si>
-    <t>Chittorgarh, Udaipur, Banswara</t>
-  </si>
-  <si>
     <t>Tamil Nadu</t>
   </si>
   <si>
@@ -859,13 +850,166 @@
   </si>
   <si>
     <t>"Longding"</t>
+  </si>
+  <si>
+    <t>Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>Y.S.R. Kadapa</t>
+  </si>
+  <si>
+    <t>Cuddapah</t>
+  </si>
+  <si>
+    <t>2010 (In DLHS3 and 4 as Cuddapah)</t>
+  </si>
+  <si>
+    <t>Palwal</t>
+  </si>
+  <si>
+    <t>Faridabad</t>
+  </si>
+  <si>
+    <t>North Cachar Hills</t>
+  </si>
+  <si>
+    <t>Yadgir</t>
+  </si>
+  <si>
+    <t>Sibsagar</t>
+  </si>
+  <si>
+    <t>Kabirdham</t>
+  </si>
+  <si>
+    <t>Kawardha</t>
+  </si>
+  <si>
+    <t>Uttar Baster Kanker</t>
+  </si>
+  <si>
+    <t>Kanker</t>
+  </si>
+  <si>
+    <t>Narayanpur</t>
+  </si>
+  <si>
+    <t>Sri Potti Sriramulu Nellore</t>
+  </si>
+  <si>
+    <t>Nellore</t>
+  </si>
+  <si>
+    <t>Referred to as just Nellore in DLHS 3 and 4</t>
+  </si>
+  <si>
+    <t>Reasi</t>
+  </si>
+  <si>
+    <t>Madhya Pradesh</t>
+  </si>
+  <si>
+    <t>Ashoknagar</t>
+  </si>
+  <si>
+    <t>Guna</t>
+  </si>
+  <si>
+    <t>Anuppur</t>
+  </si>
+  <si>
+    <t>Shahdol</t>
+  </si>
+  <si>
+    <t>Burhanpur</t>
+  </si>
+  <si>
+    <t>East Nimar</t>
+  </si>
+  <si>
+    <t>Punjab</t>
+  </si>
+  <si>
+    <t>Shahid Bhagat Singh Nagar</t>
+  </si>
+  <si>
+    <t>Nawanshahr</t>
+  </si>
+  <si>
+    <t>Chittaurgarh, Udaipur, Banswara</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>Mahamaya Nagar</t>
+  </si>
+  <si>
+    <t>Hathras</t>
+  </si>
+  <si>
+    <t>only nfhs5 has in as mahamaya nagar</t>
+  </si>
+  <si>
+    <t>south salmara mancachar</t>
+  </si>
+  <si>
+    <t>Gariyaband</t>
+  </si>
+  <si>
+    <t>Kodagaon</t>
+  </si>
+  <si>
+    <t>Dantewada</t>
+  </si>
+  <si>
+    <t>Aravali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devbhumi Dwarka </t>
+  </si>
+  <si>
+    <t>Jamnagar</t>
+  </si>
+  <si>
+    <t>Charkhi Dadri</t>
+  </si>
+  <si>
+    <t>Agar Malwa</t>
+  </si>
+  <si>
+    <t>Shajapur</t>
+  </si>
+  <si>
+    <t>Fazilka</t>
+  </si>
+  <si>
+    <t>Firozpur</t>
+  </si>
+  <si>
+    <t>Pathankot</t>
+  </si>
+  <si>
+    <t>Gurdaspur</t>
+  </si>
+  <si>
+    <t>Bhadradri Kothagudem</t>
+  </si>
+  <si>
+    <t>Khammam</t>
+  </si>
+  <si>
+    <t>Jagtial</t>
+  </si>
+  <si>
+    <t>Jangoan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -880,6 +1024,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -902,9 +1052,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,6 +1071,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1219,10 +1374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575372E9-62C3-4E49-80CB-916BD0797513}">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1249,30 +1404,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>271</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>272</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>2012</v>
+        <v>273</v>
+      </c>
+      <c r="D2" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
+        <v>271</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>285</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>2014</v>
+        <v>286</v>
+      </c>
+      <c r="D3" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1280,13 +1435,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D4">
-        <v>2015</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1294,13 +1449,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D5">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1308,13 +1463,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>2017</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1322,13 +1477,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>2017</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1336,13 +1491,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1350,13 +1505,13 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D9">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1364,10 +1519,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10">
         <v>2018</v>
@@ -1375,55 +1530,55 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D11">
-        <v>2010</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D12">
-        <v>2015</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>277</v>
       </c>
       <c r="D13">
-        <v>2015</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D14">
         <v>2015</v>
@@ -1431,13 +1586,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>279</v>
       </c>
       <c r="D15">
         <v>2015</v>
@@ -1445,13 +1600,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D16">
         <v>2015</v>
@@ -1459,41 +1614,41 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D17">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D18">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D19">
         <v>2016</v>
@@ -1501,69 +1656,63 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D20">
-        <v>2012</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>304</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21">
-        <v>2012</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22">
-        <v>2012</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D23">
-        <v>2012</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D24">
         <v>2012</v>
@@ -1571,27 +1720,27 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D25">
-        <v>2020</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D26">
         <v>2012</v>
@@ -1599,13 +1748,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D27">
         <v>2012</v>
@@ -1613,13 +1762,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D28">
         <v>2012</v>
@@ -1627,139 +1776,130 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D29">
-        <v>2012</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>306</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D30">
-        <v>2007</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>284</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D31">
-        <v>2013</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D32">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>307</v>
       </c>
       <c r="D33">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="D34">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>280</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35">
-        <v>2013</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>305</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36">
-        <v>2013</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>282</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37">
-        <v>2016</v>
+        <v>283</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="D38">
         <v>2007</v>
@@ -1767,111 +1907,111 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>308</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D39">
-        <v>2007</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="C40" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D40">
-        <v>2007</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C41" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D41">
-        <v>2007</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C42" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="D42">
-        <v>2009</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="D43">
-        <v>2020</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>309</v>
       </c>
       <c r="C44" t="s">
-        <v>92</v>
+        <v>310</v>
       </c>
       <c r="D44">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="D45">
-        <v>2016</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>311</v>
       </c>
       <c r="C46" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="D46">
         <v>2016</v>
@@ -1879,195 +2019,192 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>275</v>
       </c>
       <c r="C47" t="s">
-        <v>99</v>
-      </c>
-      <c r="D47">
-        <v>2016</v>
+        <v>276</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="D48">
-        <v>2016</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="C49" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="D49">
-        <v>2016</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B50" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C50" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="D50">
-        <v>2016</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="C51" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="D51">
-        <v>2016</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>278</v>
       </c>
       <c r="C52" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="D52">
-        <v>2012</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="B53" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="C53" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="D53">
-        <v>2012</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>289</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>290</v>
       </c>
       <c r="C54" t="s">
-        <v>116</v>
+        <v>291</v>
       </c>
       <c r="D54">
-        <v>2012</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>108</v>
+        <v>289</v>
       </c>
       <c r="B55" t="s">
-        <v>112</v>
+        <v>294</v>
       </c>
       <c r="C55" t="s">
-        <v>117</v>
+        <v>295</v>
       </c>
       <c r="D55">
-        <v>2012</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>108</v>
+        <v>289</v>
       </c>
       <c r="B56" t="s">
-        <v>113</v>
+        <v>312</v>
       </c>
       <c r="C56" t="s">
-        <v>117</v>
+        <v>313</v>
       </c>
       <c r="D56">
-        <v>2012</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>108</v>
+        <v>289</v>
       </c>
       <c r="B57" t="s">
-        <v>114</v>
+        <v>292</v>
       </c>
       <c r="C57" t="s">
-        <v>118</v>
+        <v>293</v>
       </c>
       <c r="D57">
-        <v>2012</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="C58" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="D58">
-        <v>2008</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="B59" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="C59" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="D59">
-        <v>2009</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B60" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="C60" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="D60">
         <v>2016</v>
@@ -2075,13 +2212,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B61" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="C61" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="D61">
         <v>2016</v>
@@ -2089,13 +2226,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="C62" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="D62">
         <v>2016</v>
@@ -2103,13 +2240,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="C63" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="D63">
         <v>2016</v>
@@ -2117,13 +2254,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B64" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="D64">
         <v>2016</v>
@@ -2131,13 +2268,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B65" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="C65" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="D65">
         <v>2016</v>
@@ -2145,167 +2282,167 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B66" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="C66" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="D66">
-        <v>2016</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B67" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="C67" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="D67">
-        <v>2016</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="C68" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="D68">
-        <v>2016</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B69" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="C69" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="D69">
-        <v>2016</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B70" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="C70" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="D70">
-        <v>2016</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B71" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="C71" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="D71">
-        <v>2016</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>126</v>
-      </c>
-      <c r="B72" t="s">
-        <v>142</v>
+        <v>296</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>297</v>
       </c>
       <c r="C72" t="s">
-        <v>134</v>
+        <v>298</v>
       </c>
       <c r="D72">
-        <v>2016</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>126</v>
-      </c>
-      <c r="B73" t="s">
-        <v>143</v>
+        <v>296</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="C73" t="s">
-        <v>144</v>
+        <v>317</v>
       </c>
       <c r="D73">
-        <v>2016</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>126</v>
-      </c>
-      <c r="B74" t="s">
-        <v>145</v>
+        <v>296</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>314</v>
       </c>
       <c r="C74" t="s">
-        <v>146</v>
+        <v>315</v>
       </c>
       <c r="D74">
-        <v>2016</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B75" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="C75" t="s">
-        <v>146</v>
+        <v>299</v>
       </c>
       <c r="D75">
-        <v>2016</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B76" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="C76" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="D76">
-        <v>2016</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B77" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="C77" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="D77">
         <v>2016</v>
@@ -2313,13 +2450,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="B78" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="C78" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="D78">
         <v>2016</v>
@@ -2327,13 +2464,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="B79" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="C79" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="D79">
         <v>2016</v>
@@ -2341,13 +2478,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="B80" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="C80" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="D80">
         <v>2016</v>
@@ -2355,13 +2492,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C81" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="D81">
         <v>2016</v>
@@ -2369,239 +2506,502 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="B82" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="C82" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="D82">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="B83" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
       <c r="C83" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="D83">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="B84" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="C84" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="D84">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="B85" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="C85" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
       <c r="D85">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="B86" t="s">
-        <v>164</v>
+        <v>318</v>
       </c>
       <c r="C86" t="s">
-        <v>165</v>
-      </c>
-      <c r="D86">
-        <v>2014</v>
+        <v>319</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="B87" t="s">
-        <v>169</v>
+        <v>321</v>
       </c>
       <c r="C87" t="s">
-        <v>170</v>
-      </c>
-      <c r="D87" t="s">
-        <v>171</v>
+        <v>131</v>
+      </c>
+      <c r="D87">
+        <v>2016</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="B88" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="C88" t="s">
-        <v>170</v>
+        <v>131</v>
       </c>
       <c r="D88">
-        <v>2006</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>174</v>
+        <v>123</v>
       </c>
       <c r="B89" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="C89" t="s">
-        <v>180</v>
+        <v>131</v>
       </c>
       <c r="D89">
-        <v>2006</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>174</v>
+        <v>123</v>
       </c>
       <c r="B90" t="s">
-        <v>176</v>
+        <v>139</v>
       </c>
       <c r="C90" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="D90">
-        <v>2006</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>123</v>
       </c>
       <c r="B91" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="C91" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="D91">
-        <v>2006</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>174</v>
+        <v>123</v>
       </c>
       <c r="B92" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
       <c r="C92" t="s">
-        <v>179</v>
+        <v>143</v>
       </c>
       <c r="D92">
-        <v>2006</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>123</v>
       </c>
       <c r="B93" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="C93" t="s">
-        <v>188</v>
+        <v>143</v>
       </c>
       <c r="D93">
-        <v>2006</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>174</v>
+        <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>183</v>
+        <v>145</v>
       </c>
       <c r="C94" t="s">
-        <v>189</v>
+        <v>147</v>
       </c>
       <c r="D94">
-        <v>2006</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>174</v>
+        <v>123</v>
       </c>
       <c r="B95" t="s">
-        <v>184</v>
+        <v>146</v>
       </c>
       <c r="C95" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
       <c r="D95">
-        <v>2006</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="B96" t="s">
-        <v>185</v>
+        <v>149</v>
       </c>
       <c r="C96" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
       <c r="D96">
-        <v>2006</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>190</v>
+        <v>148</v>
       </c>
       <c r="B97" t="s">
-        <v>192</v>
+        <v>150</v>
       </c>
       <c r="C97" t="s">
-        <v>194</v>
+        <v>153</v>
       </c>
       <c r="D97">
-        <v>2012</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>148</v>
+      </c>
+      <c r="B98" t="s">
+        <v>151</v>
+      </c>
+      <c r="C98" t="s">
+        <v>153</v>
+      </c>
+      <c r="D98">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>148</v>
+      </c>
+      <c r="B99" t="s">
+        <v>152</v>
+      </c>
+      <c r="C99" t="s">
+        <v>154</v>
+      </c>
+      <c r="D99">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>300</v>
+      </c>
+      <c r="B100" t="s">
+        <v>301</v>
+      </c>
+      <c r="C100" t="s">
+        <v>302</v>
+      </c>
+      <c r="D100" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>156</v>
+      </c>
+      <c r="B101" t="s">
+        <v>157</v>
+      </c>
+      <c r="C101" t="s">
+        <v>164</v>
+      </c>
+      <c r="D101">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>156</v>
+      </c>
+      <c r="B102" t="s">
+        <v>158</v>
+      </c>
+      <c r="C102" t="s">
+        <v>164</v>
+      </c>
+      <c r="D102">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>156</v>
+      </c>
+      <c r="B103" t="s">
+        <v>159</v>
+      </c>
+      <c r="C103" t="s">
+        <v>165</v>
+      </c>
+      <c r="D103">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>156</v>
+      </c>
+      <c r="B104" t="s">
+        <v>160</v>
+      </c>
+      <c r="C104" t="s">
+        <v>163</v>
+      </c>
+      <c r="D104">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>156</v>
+      </c>
+      <c r="B105" t="s">
+        <v>161</v>
+      </c>
+      <c r="C105" t="s">
+        <v>162</v>
+      </c>
+      <c r="D105">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>170</v>
+      </c>
+      <c r="B106" t="s">
+        <v>166</v>
+      </c>
+      <c r="C106" t="s">
+        <v>167</v>
+      </c>
+      <c r="D106" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>170</v>
+      </c>
+      <c r="B107" t="s">
+        <v>169</v>
+      </c>
+      <c r="C107" t="s">
+        <v>167</v>
+      </c>
+      <c r="D107">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>171</v>
+      </c>
+      <c r="B108" t="s">
+        <v>172</v>
+      </c>
+      <c r="C108" t="s">
+        <v>177</v>
+      </c>
+      <c r="D108">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>171</v>
+      </c>
+      <c r="B109" t="s">
+        <v>288</v>
+      </c>
+      <c r="C109" t="s">
+        <v>178</v>
+      </c>
+      <c r="D109">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>171</v>
+      </c>
+      <c r="B110" t="s">
+        <v>174</v>
+      </c>
+      <c r="C110" t="s">
+        <v>176</v>
+      </c>
+      <c r="D110">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>171</v>
+      </c>
+      <c r="B111" t="s">
+        <v>175</v>
+      </c>
+      <c r="C111" t="s">
+        <v>176</v>
+      </c>
+      <c r="D111">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>171</v>
+      </c>
+      <c r="B112" t="s">
+        <v>179</v>
+      </c>
+      <c r="C112" t="s">
+        <v>185</v>
+      </c>
+      <c r="D112">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>171</v>
+      </c>
+      <c r="B113" t="s">
+        <v>180</v>
+      </c>
+      <c r="C113" t="s">
+        <v>186</v>
+      </c>
+      <c r="D113">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>171</v>
+      </c>
+      <c r="B114" t="s">
+        <v>181</v>
+      </c>
+      <c r="C114" t="s">
+        <v>183</v>
+      </c>
+      <c r="D114">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>171</v>
+      </c>
+      <c r="B115" t="s">
+        <v>182</v>
+      </c>
+      <c r="C115" t="s">
+        <v>184</v>
+      </c>
+      <c r="D115">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>187</v>
+      </c>
+      <c r="B116" t="s">
+        <v>189</v>
+      </c>
+      <c r="C116" t="s">
+        <v>191</v>
+      </c>
+      <c r="D116">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>187</v>
+      </c>
+      <c r="B117" t="s">
+        <v>188</v>
+      </c>
+      <c r="C117" t="s">
         <v>190</v>
       </c>
-      <c r="B98" t="s">
-        <v>191</v>
-      </c>
-      <c r="C98" t="s">
-        <v>193</v>
-      </c>
-      <c r="D98">
+      <c r="D117">
         <v>2012</v>
       </c>
     </row>
@@ -2614,8 +3014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F736FB1-4867-5049-BBBA-0253BCC87D95}">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD58"/>
+    <sheetView topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2636,1360 +3036,1360 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" t="s">
         <v>195</v>
-      </c>
-      <c r="D4" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D13" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D14" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D16" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D17" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D19" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D20" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D21" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D22" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D23" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D24" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D25" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D26" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D27" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D29" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D30" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D31" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D32" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D33" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D34" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D35" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D36" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D37" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D38" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C39" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D39" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D40" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C41" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D41" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C42" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D42" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C43" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D43" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C44" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D44" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C45" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D45" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C46" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D46" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C47" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D47" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C48" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D48" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C49" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D49" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B50" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C50" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D50" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C51" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D51" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C52" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D52" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B53" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C53" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D53" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C54" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D54" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B55" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C55" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D55" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B56" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C56" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D56" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B57" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C57" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D57" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B58" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C58" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D58" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B59" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C59" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D59" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B60" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C60" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D60" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B61" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C61" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D61" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C62" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D62" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C63" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D63" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B64" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C64" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D64" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B65" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C65" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D65" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B66" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C66" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D66" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B67" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C67" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D67" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C68" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D68" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B69" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C69" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D69" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B70" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C70" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D70" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B71" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C71" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D71" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B72" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C72" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D72" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B73" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C73" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D73" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B74" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C74" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D74" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B75" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C75" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D75" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B76" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C76" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D76" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B77" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C77" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D77" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B78" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C78" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D78" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B79" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C79" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D79" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B80" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C80" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D80" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C81" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D81" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B82" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C82" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D82" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B83" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C83" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D83" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B84" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C84" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D84" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B85" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C85" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D85" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B86" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C86" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D86" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B87" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C87" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D87" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B88" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C88" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D88" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B89" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C89" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D89" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B90" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C90" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D90" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B91" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C91" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D91" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B92" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C92" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D92" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B93" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C93" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D93" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B94" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C94" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D94" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B95" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C95" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D95" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B96" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C96" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D96" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B97" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C97" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D97" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B98" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C98" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D98" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -3998,6 +4398,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009FE99232C2A610489C05CA2A95C6B0DC" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="99e3d855f4612a477f80c26c84225e60">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="748de206-7911-403a-93a2-ff3feb5ad88e" xmlns:ns3="d391a701-1e72-4a9c-8e27-32ae852ac85b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9d24ec2972380c9becf470258562e41c" ns2:_="" ns3:_="">
     <xsd:import namespace="748de206-7911-403a-93a2-ff3feb5ad88e"/>
@@ -4228,19 +4637,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA9CD780-B0BD-40BC-A1F0-B37A41579C99}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FDE1080-05E2-40DC-AFCB-2FF0EFA9E9BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FDE1080-05E2-40DC-AFCB-2FF0EFA9E9BF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA9CD780-B0BD-40BC-A1F0-B37A41579C99}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="748de206-7911-403a-93a2-ff3feb5ad88e"/>
+    <ds:schemaRef ds:uri="d391a701-1e72-4a9c-8e27-32ae852ac85b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating state_district coding for harmonization at district level
</commit_message>
<xml_diff>
--- a/District_Changes.xlsx
+++ b/District_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill.sharepoint.com/sites/PROSPERED_Group/Shared Documents/General/CIHR RSBY India/data/Linking code and CSVs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="658" documentId="8_{B95B0D2E-E9D4-8740-A922-149F5228A517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C4F2AE9-04FA-E840-9224-79CFA44E1815}"/>
+  <xr:revisionPtr revIDLastSave="762" documentId="8_{B95B0D2E-E9D4-8740-A922-149F5228A517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AE84788-8246-9B43-853C-B88E4114EE09}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1620" windowWidth="33620" windowHeight="19380" xr2:uid="{D1D00CCF-82AB-6D4D-9728-F84D718C5775}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{D1D00CCF-82AB-6D4D-9728-F84D718C5775}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="350">
   <si>
     <t>State</t>
   </si>
@@ -219,9 +219,6 @@
     <t>Aravalli</t>
   </si>
   <si>
-    <t>Sabarkantha</t>
-  </si>
-  <si>
     <t>Botad</t>
   </si>
   <si>
@@ -468,9 +465,6 @@
     <t>Vikarabad</t>
   </si>
   <si>
-    <t>Ranga Reddy</t>
-  </si>
-  <si>
     <t>Medchal-Malkajgiri</t>
   </si>
   <si>
@@ -480,9 +474,6 @@
     <t>Jogulamba</t>
   </si>
   <si>
-    <t>Mahabubnagar</t>
-  </si>
-  <si>
     <t>Tripura</t>
   </si>
   <si>
@@ -531,9 +522,6 @@
     <t>Darjeeling</t>
   </si>
   <si>
-    <t>Bardhaman</t>
-  </si>
-  <si>
     <t>Paschim Medinipur</t>
   </si>
   <si>
@@ -1003,6 +991,102 @@
   </si>
   <si>
     <t>Jangoan</t>
+  </si>
+  <si>
+    <t>Jayashankar Bhupalapally</t>
+  </si>
+  <si>
+    <t>Jogulamba Gadwal</t>
+  </si>
+  <si>
+    <t>Komaram Bheem Asifabad</t>
+  </si>
+  <si>
+    <t>Rangareddy</t>
+  </si>
+  <si>
+    <t>Sangareddy</t>
+  </si>
+  <si>
+    <t>Medak</t>
+  </si>
+  <si>
+    <t>Siddipet</t>
+  </si>
+  <si>
+    <t>Suryapet</t>
+  </si>
+  <si>
+    <t>Mahbubnagar</t>
+  </si>
+  <si>
+    <t>Wanaparthy</t>
+  </si>
+  <si>
+    <t>Warangal Urban</t>
+  </si>
+  <si>
+    <t>Sepahijala</t>
+  </si>
+  <si>
+    <t>Amethi</t>
+  </si>
+  <si>
+    <t>Sultanpur</t>
+  </si>
+  <si>
+    <t>Hapur</t>
+  </si>
+  <si>
+    <t>Ghaziabad</t>
+  </si>
+  <si>
+    <t>Sambhal</t>
+  </si>
+  <si>
+    <t>Moradabad</t>
+  </si>
+  <si>
+    <t>Shamli</t>
+  </si>
+  <si>
+    <t>Muzaffarnagar </t>
+  </si>
+  <si>
+    <t>Paschim Barddhaman</t>
+  </si>
+  <si>
+    <t>Purba Barddhaman</t>
+  </si>
+  <si>
+    <t>Barddhaman</t>
+  </si>
+  <si>
+    <t>Sabar Kantha</t>
+  </si>
+  <si>
+    <t>Kanshiram Nagar</t>
+  </si>
+  <si>
+    <t>Etah</t>
+  </si>
+  <si>
+    <t>Shupiyan</t>
+  </si>
+  <si>
+    <t>Bandipore</t>
+  </si>
+  <si>
+    <t>Alirajpur</t>
+  </si>
+  <si>
+    <t>Jhabua</t>
+  </si>
+  <si>
+    <t>Singrauli</t>
+  </si>
+  <si>
+    <t>Sidhi</t>
   </si>
 </sst>
 </file>
@@ -1071,10 +1155,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1374,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575372E9-62C3-4E49-80CB-916BD0797513}">
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1404,30 +1484,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C3" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1564,7 +1644,7 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D13">
         <v>2010</v>
@@ -1592,7 +1672,7 @@
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D15">
         <v>2015</v>
@@ -1673,7 +1753,7 @@
         <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C21" t="s">
         <v>30</v>
@@ -1687,7 +1767,7 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1793,7 +1873,7 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C30" t="s">
         <v>52</v>
@@ -1807,7 +1887,7 @@
         <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C31" t="s">
         <v>52</v>
@@ -1838,7 +1918,7 @@
         <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D33">
         <v>2012</v>
@@ -1863,10 +1943,10 @@
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C35" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1874,7 +1954,7 @@
         <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C36" t="s">
         <v>44</v>
@@ -1885,10 +1965,10 @@
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C37" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1910,10 +1990,10 @@
         <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C39" t="s">
-        <v>60</v>
+        <v>341</v>
       </c>
       <c r="D39">
         <v>2013</v>
@@ -1924,10 +2004,10 @@
         <v>56</v>
       </c>
       <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" t="s">
         <v>61</v>
-      </c>
-      <c r="C40" t="s">
-        <v>62</v>
       </c>
       <c r="D40">
         <v>2013</v>
@@ -1938,10 +2018,10 @@
         <v>56</v>
       </c>
       <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
         <v>63</v>
-      </c>
-      <c r="C41" t="s">
-        <v>64</v>
       </c>
       <c r="D41">
         <v>2013</v>
@@ -1952,10 +2032,10 @@
         <v>56</v>
       </c>
       <c r="B42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" t="s">
         <v>65</v>
-      </c>
-      <c r="C42" t="s">
-        <v>66</v>
       </c>
       <c r="D42">
         <v>2013</v>
@@ -1966,10 +2046,10 @@
         <v>56</v>
       </c>
       <c r="B43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" t="s">
         <v>67</v>
-      </c>
-      <c r="C43" t="s">
-        <v>68</v>
       </c>
       <c r="D43">
         <v>2013</v>
@@ -1980,10 +2060,10 @@
         <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C44" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D44">
         <v>2013</v>
@@ -1994,10 +2074,10 @@
         <v>56</v>
       </c>
       <c r="B45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" t="s">
         <v>69</v>
-      </c>
-      <c r="C45" t="s">
-        <v>70</v>
       </c>
       <c r="D45">
         <v>2013</v>
@@ -2005,13 +2085,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B46" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D46">
         <v>2016</v>
@@ -2019,24 +2099,24 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B47" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C47" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" t="s">
         <v>74</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>75</v>
-      </c>
-      <c r="C48" t="s">
-        <v>76</v>
       </c>
       <c r="D48">
         <v>2007</v>
@@ -2044,13 +2124,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B49" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" t="s">
         <v>77</v>
-      </c>
-      <c r="C49" t="s">
-        <v>78</v>
       </c>
       <c r="D49">
         <v>2007</v>
@@ -2058,13 +2138,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" t="s">
         <v>79</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>80</v>
-      </c>
-      <c r="C50" t="s">
-        <v>81</v>
       </c>
       <c r="D50">
         <v>2007</v>
@@ -2072,13 +2152,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B51" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" t="s">
         <v>82</v>
-      </c>
-      <c r="C51" t="s">
-        <v>83</v>
       </c>
       <c r="D51">
         <v>2007</v>
@@ -2086,13 +2166,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D52">
         <v>2009</v>
@@ -2100,13 +2180,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" t="s">
         <v>86</v>
-      </c>
-      <c r="C53" t="s">
-        <v>87</v>
       </c>
       <c r="D53">
         <v>2020</v>
@@ -2114,13 +2194,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B54" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C54" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D54">
         <v>2003</v>
@@ -2128,13 +2208,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B55" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C55" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D55">
         <v>2003</v>
@@ -2142,13 +2222,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B56" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C56" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D56">
         <v>2013</v>
@@ -2156,69 +2236,69 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B57" t="s">
-        <v>292</v>
+        <v>346</v>
       </c>
       <c r="C57" t="s">
-        <v>293</v>
+        <v>347</v>
       </c>
       <c r="D57">
-        <v>2003</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>88</v>
+        <v>285</v>
       </c>
       <c r="B58" t="s">
-        <v>89</v>
+        <v>348</v>
       </c>
       <c r="C58" t="s">
-        <v>90</v>
+        <v>349</v>
       </c>
       <c r="D58">
-        <v>2014</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>91</v>
+        <v>285</v>
       </c>
       <c r="B59" t="s">
-        <v>92</v>
+        <v>288</v>
       </c>
       <c r="C59" t="s">
-        <v>93</v>
+        <v>289</v>
       </c>
       <c r="D59">
-        <v>2016</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B60" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C60" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D60">
-        <v>2016</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>90</v>
+      </c>
+      <c r="B61" t="s">
         <v>91</v>
       </c>
-      <c r="B61" t="s">
-        <v>96</v>
-      </c>
       <c r="C61" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D61">
         <v>2016</v>
@@ -2226,13 +2306,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B62" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C62" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D62">
         <v>2016</v>
@@ -2240,13 +2320,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B63" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C63" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D63">
         <v>2016</v>
@@ -2254,13 +2334,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B64" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C64" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D64">
         <v>2016</v>
@@ -2268,13 +2348,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B65" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C65" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D65">
         <v>2016</v>
@@ -2282,41 +2362,41 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B66" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C66" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D66">
-        <v>2012</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B67" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C67" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D67">
-        <v>2012</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>105</v>
+      </c>
+      <c r="B68" t="s">
         <v>106</v>
       </c>
-      <c r="B68" t="s">
-        <v>109</v>
-      </c>
       <c r="C68" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D68">
         <v>2012</v>
@@ -2324,13 +2404,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B69" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C69" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D69">
         <v>2012</v>
@@ -2338,13 +2418,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B70" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C70" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D70">
         <v>2012</v>
@@ -2352,13 +2432,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B71" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C71" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D71">
         <v>2012</v>
@@ -2366,111 +2446,111 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>296</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>297</v>
+        <v>105</v>
+      </c>
+      <c r="B72" t="s">
+        <v>110</v>
       </c>
       <c r="C72" t="s">
-        <v>298</v>
+        <v>114</v>
       </c>
       <c r="D72">
-        <v>2008</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>296</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>316</v>
+        <v>105</v>
+      </c>
+      <c r="B73" t="s">
+        <v>111</v>
       </c>
       <c r="C73" t="s">
-        <v>317</v>
+        <v>115</v>
       </c>
       <c r="D73">
-        <v>2011</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>314</v>
+        <v>293</v>
       </c>
       <c r="C74" t="s">
-        <v>315</v>
+        <v>294</v>
       </c>
       <c r="D74">
-        <v>2011</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>117</v>
-      </c>
-      <c r="B75" t="s">
-        <v>118</v>
+        <v>292</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>312</v>
       </c>
       <c r="C75" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="D75">
-        <v>2008</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>119</v>
-      </c>
-      <c r="B76" t="s">
-        <v>121</v>
+        <v>292</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>310</v>
       </c>
       <c r="C76" t="s">
-        <v>122</v>
+        <v>311</v>
       </c>
       <c r="D76">
-        <v>2009</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B77" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C77" t="s">
-        <v>124</v>
+        <v>295</v>
       </c>
       <c r="D77">
-        <v>2016</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B78" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C78" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D78">
-        <v>2016</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>122</v>
+      </c>
+      <c r="B79" t="s">
         <v>123</v>
       </c>
-      <c r="B79" t="s">
-        <v>126</v>
-      </c>
       <c r="C79" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D79">
         <v>2016</v>
@@ -2478,13 +2558,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>122</v>
+      </c>
+      <c r="B80" t="s">
+        <v>320</v>
+      </c>
+      <c r="C80" t="s">
         <v>123</v>
-      </c>
-      <c r="B80" t="s">
-        <v>127</v>
-      </c>
-      <c r="C80" t="s">
-        <v>124</v>
       </c>
       <c r="D80">
         <v>2016</v>
@@ -2492,13 +2572,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>122</v>
+      </c>
+      <c r="B81" t="s">
+        <v>125</v>
+      </c>
+      <c r="C81" t="s">
         <v>123</v>
-      </c>
-      <c r="B81" t="s">
-        <v>128</v>
-      </c>
-      <c r="C81" t="s">
-        <v>129</v>
       </c>
       <c r="D81">
         <v>2016</v>
@@ -2506,13 +2586,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>122</v>
+      </c>
+      <c r="B82" t="s">
+        <v>126</v>
+      </c>
+      <c r="C82" t="s">
         <v>123</v>
-      </c>
-      <c r="B82" t="s">
-        <v>130</v>
-      </c>
-      <c r="C82" t="s">
-        <v>131</v>
       </c>
       <c r="D82">
         <v>2016</v>
@@ -2520,13 +2600,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B83" t="s">
-        <v>320</v>
+        <v>127</v>
       </c>
       <c r="C83" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D83">
         <v>2016</v>
@@ -2534,13 +2614,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B84" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C84" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D84">
         <v>2016</v>
@@ -2548,13 +2628,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B85" t="s">
+        <v>316</v>
+      </c>
+      <c r="C85" t="s">
         <v>134</v>
-      </c>
-      <c r="C85" t="s">
-        <v>135</v>
       </c>
       <c r="D85">
         <v>2016</v>
@@ -2562,24 +2642,27 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B86" t="s">
-        <v>318</v>
+        <v>132</v>
       </c>
       <c r="C86" t="s">
-        <v>319</v>
+        <v>134</v>
+      </c>
+      <c r="D86">
+        <v>2016</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B87" t="s">
-        <v>321</v>
+        <v>133</v>
       </c>
       <c r="C87" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D87">
         <v>2016</v>
@@ -2587,13 +2670,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B88" t="s">
-        <v>137</v>
+        <v>314</v>
       </c>
       <c r="C88" t="s">
-        <v>131</v>
+        <v>315</v>
       </c>
       <c r="D88">
         <v>2016</v>
@@ -2601,13 +2684,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B89" t="s">
-        <v>138</v>
+        <v>317</v>
       </c>
       <c r="C89" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D89">
         <v>2016</v>
@@ -2615,13 +2698,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B90" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C90" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D90">
         <v>2016</v>
@@ -2629,13 +2712,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B91" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C91" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D91">
         <v>2016</v>
@@ -2643,13 +2726,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B92" t="s">
-        <v>142</v>
+        <v>328</v>
       </c>
       <c r="C92" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="D92">
         <v>2016</v>
@@ -2657,13 +2740,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B93" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C93" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="D93">
         <v>2016</v>
@@ -2671,13 +2754,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B94" t="s">
-        <v>145</v>
+        <v>318</v>
       </c>
       <c r="C94" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="D94">
         <v>2016</v>
@@ -2685,13 +2768,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B95" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C95" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D95">
         <v>2016</v>
@@ -2699,13 +2782,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="B96" t="s">
-        <v>149</v>
+        <v>325</v>
       </c>
       <c r="C96" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="D96">
         <v>2016</v>
@@ -2713,13 +2796,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="B97" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C97" t="s">
-        <v>153</v>
+        <v>321</v>
       </c>
       <c r="D97">
         <v>2016</v>
@@ -2727,13 +2810,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="B98" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C98" t="s">
-        <v>153</v>
+        <v>321</v>
       </c>
       <c r="D98">
         <v>2016</v>
@@ -2741,13 +2824,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="B99" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C99" t="s">
-        <v>154</v>
+        <v>326</v>
       </c>
       <c r="D99">
         <v>2016</v>
@@ -2755,253 +2838,435 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>300</v>
+        <v>122</v>
       </c>
       <c r="B100" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="C100" t="s">
-        <v>302</v>
-      </c>
-      <c r="D100" t="s">
-        <v>303</v>
+        <v>326</v>
+      </c>
+      <c r="D100">
+        <v>2016</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="B101" t="s">
-        <v>157</v>
+        <v>327</v>
       </c>
       <c r="C101" t="s">
-        <v>164</v>
+        <v>326</v>
       </c>
       <c r="D101">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="B102" t="s">
-        <v>158</v>
+        <v>322</v>
       </c>
       <c r="C102" t="s">
-        <v>164</v>
+        <v>323</v>
       </c>
       <c r="D102">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="B103" t="s">
-        <v>159</v>
+        <v>324</v>
       </c>
       <c r="C103" t="s">
-        <v>165</v>
+        <v>323</v>
       </c>
       <c r="D103">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B104" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C104" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D104">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B105" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="C105" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D105">
-        <v>2014</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="B106" t="s">
-        <v>166</v>
+        <v>329</v>
       </c>
       <c r="C106" t="s">
-        <v>167</v>
-      </c>
-      <c r="D106" t="s">
-        <v>168</v>
+        <v>150</v>
+      </c>
+      <c r="D106">
+        <v>2016</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="B107" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="C107" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="D107">
-        <v>2006</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>171</v>
+        <v>296</v>
       </c>
       <c r="B108" t="s">
-        <v>172</v>
+        <v>297</v>
       </c>
       <c r="C108" t="s">
-        <v>177</v>
-      </c>
-      <c r="D108">
-        <v>2006</v>
+        <v>298</v>
+      </c>
+      <c r="D108" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>171</v>
+        <v>296</v>
       </c>
       <c r="B109" t="s">
-        <v>288</v>
+        <v>332</v>
       </c>
       <c r="C109" t="s">
-        <v>178</v>
+        <v>333</v>
       </c>
       <c r="D109">
-        <v>2006</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>171</v>
+        <v>296</v>
       </c>
       <c r="B110" t="s">
-        <v>174</v>
+        <v>334</v>
       </c>
       <c r="C110" t="s">
-        <v>176</v>
+        <v>335</v>
       </c>
       <c r="D110">
-        <v>2006</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>171</v>
+        <v>296</v>
       </c>
       <c r="B111" t="s">
-        <v>175</v>
+        <v>336</v>
       </c>
       <c r="C111" t="s">
-        <v>176</v>
+        <v>337</v>
       </c>
       <c r="D111">
-        <v>2006</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>171</v>
+        <v>296</v>
       </c>
       <c r="B112" t="s">
-        <v>179</v>
+        <v>342</v>
       </c>
       <c r="C112" t="s">
-        <v>185</v>
+        <v>343</v>
       </c>
       <c r="D112">
-        <v>2006</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>171</v>
+        <v>296</v>
       </c>
       <c r="B113" t="s">
-        <v>180</v>
+        <v>330</v>
       </c>
       <c r="C113" t="s">
-        <v>186</v>
+        <v>331</v>
       </c>
       <c r="D113">
-        <v>2006</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="B114" t="s">
-        <v>181</v>
+        <v>338</v>
       </c>
       <c r="C114" t="s">
-        <v>183</v>
+        <v>340</v>
       </c>
       <c r="D114">
-        <v>2006</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="B115" t="s">
-        <v>182</v>
+        <v>339</v>
       </c>
       <c r="C115" t="s">
-        <v>184</v>
+        <v>340</v>
       </c>
       <c r="D115">
-        <v>2006</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="B116" t="s">
-        <v>189</v>
+        <v>156</v>
       </c>
       <c r="C116" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
       <c r="D116">
-        <v>2012</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>153</v>
+      </c>
+      <c r="B117" t="s">
+        <v>157</v>
+      </c>
+      <c r="C117" t="s">
+        <v>160</v>
+      </c>
+      <c r="D117">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>153</v>
+      </c>
+      <c r="B118" t="s">
+        <v>158</v>
+      </c>
+      <c r="C118" t="s">
+        <v>159</v>
+      </c>
+      <c r="D118">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>166</v>
+      </c>
+      <c r="B119" t="s">
+        <v>162</v>
+      </c>
+      <c r="C119" t="s">
+        <v>163</v>
+      </c>
+      <c r="D119" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>166</v>
+      </c>
+      <c r="B120" t="s">
+        <v>165</v>
+      </c>
+      <c r="C120" t="s">
+        <v>163</v>
+      </c>
+      <c r="D120">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>167</v>
+      </c>
+      <c r="B121" t="s">
+        <v>168</v>
+      </c>
+      <c r="C121" t="s">
+        <v>173</v>
+      </c>
+      <c r="D121">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>167</v>
+      </c>
+      <c r="B122" t="s">
+        <v>284</v>
+      </c>
+      <c r="C122" t="s">
+        <v>174</v>
+      </c>
+      <c r="D122">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>167</v>
+      </c>
+      <c r="B123" t="s">
+        <v>170</v>
+      </c>
+      <c r="C123" t="s">
+        <v>172</v>
+      </c>
+      <c r="D123">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>167</v>
+      </c>
+      <c r="B124" t="s">
+        <v>171</v>
+      </c>
+      <c r="C124" t="s">
+        <v>172</v>
+      </c>
+      <c r="D124">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>167</v>
+      </c>
+      <c r="B125" t="s">
+        <v>175</v>
+      </c>
+      <c r="C125" t="s">
+        <v>181</v>
+      </c>
+      <c r="D125">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>167</v>
+      </c>
+      <c r="B126" t="s">
+        <v>344</v>
+      </c>
+      <c r="C126" t="s">
+        <v>182</v>
+      </c>
+      <c r="D126">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>167</v>
+      </c>
+      <c r="B127" t="s">
+        <v>177</v>
+      </c>
+      <c r="C127" t="s">
+        <v>179</v>
+      </c>
+      <c r="D127">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>167</v>
+      </c>
+      <c r="B128" t="s">
+        <v>345</v>
+      </c>
+      <c r="C128" t="s">
+        <v>180</v>
+      </c>
+      <c r="D128">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>183</v>
+      </c>
+      <c r="B129" t="s">
+        <v>185</v>
+      </c>
+      <c r="C129" t="s">
         <v>187</v>
       </c>
-      <c r="B117" t="s">
-        <v>188</v>
-      </c>
-      <c r="C117" t="s">
-        <v>190</v>
-      </c>
-      <c r="D117">
+      <c r="D129">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>183</v>
+      </c>
+      <c r="B130" t="s">
+        <v>184</v>
+      </c>
+      <c r="C130" t="s">
+        <v>186</v>
+      </c>
+      <c r="D130">
         <v>2012</v>
       </c>
     </row>
@@ -3036,1360 +3301,1360 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" t="s">
         <v>192</v>
-      </c>
-      <c r="D5" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D12" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D14" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D15" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D16" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B17" t="s">
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D17" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D18" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B19" t="s">
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D19" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B20" t="s">
         <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D20" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D21" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B22" t="s">
         <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D22" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B23" t="s">
         <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D23" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D24" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D25" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D26" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B27" t="s">
         <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D27" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B28" t="s">
         <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D28" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B29" t="s">
         <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D29" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B30" t="s">
         <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D30" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B31" t="s">
         <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D31" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D32" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D33" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D34" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D35" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D36" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D37" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D38" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D39" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D40" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D41" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D42" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D43" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C44" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D44" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D45" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D46" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C47" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D47" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C48" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D48" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C49" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D49" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C50" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D50" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B51" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C51" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D51" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C52" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D52" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C53" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D53" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C54" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D54" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B55" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C55" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D55" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C56" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D56" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C57" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D57" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C58" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D58" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C59" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D59" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C60" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D60" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B61" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C61" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D61" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B62" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C62" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D62" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C63" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D63" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B64" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C64" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D64" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B65" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C65" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D65" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C66" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D66" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B67" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C67" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D67" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C68" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D68" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C69" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D69" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B70" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C70" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D70" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B71" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C71" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D71" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B72" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C72" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D72" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B73" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C73" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D73" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B74" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C74" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D74" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B75" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C75" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D75" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B76" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C76" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D76" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B77" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C77" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D77" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B78" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C78" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D78" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B79" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C79" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D79" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B80" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C80" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D80" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B81" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C81" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D81" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B82" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C82" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D82" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B83" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C83" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D83" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B84" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C84" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D84" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B85" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C85" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D85" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B86" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C86" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D86" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B87" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C87" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D87" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B88" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C88" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D88" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B89" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C89" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D89" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B90" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C90" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D90" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B91" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C91" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D91" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B92" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C92" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D92" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B93" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C93" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D93" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B94" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C94" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D94" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B95" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C95" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D95" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B96" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C96" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D96" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B97" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C97" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D97" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B98" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C98" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D98" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>